<commit_message>
Started new potential pattern image decode
</commit_message>
<xml_diff>
--- a/API Faults Taxonomy.xlsx
+++ b/API Faults Taxonomy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wilso\OneDrive\Documents\Final Year Project\DL-BUG-FINDER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F48FF01-B751-48E5-B871-3072FB77162C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A196E8-123E-488D-B577-B364E77F7EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{50305C56-3506-426A-9490-D1BCFFFE2880}"/>
   </bookViews>
@@ -222,7 +222,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -233,6 +233,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF9BC2E6"/>
         <bgColor rgb="FF9BC2E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -248,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -268,6 +274,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,12 +592,13 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:G16"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.36328125" customWidth="1"/>
+    <col min="2" max="2" width="56.1796875" customWidth="1"/>
     <col min="3" max="3" width="16.1796875" customWidth="1"/>
     <col min="4" max="4" width="18.90625" customWidth="1"/>
     <col min="5" max="5" width="16.08984375" customWidth="1"/>
@@ -636,6 +644,7 @@
       <c r="F2" s="1">
         <v>3</v>
       </c>
+      <c r="G2" s="13"/>
     </row>
     <row r="3" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">

</xml_diff>

<commit_message>
Test files for finding/fixing
</commit_message>
<xml_diff>
--- a/API Faults Taxonomy.xlsx
+++ b/API Faults Taxonomy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barry\workspace\700\DL-BUG-FINDER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B6F24F-5889-4AA7-90A7-9AFC09602CD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33782860-FB1A-4DB8-9BD3-B95F433E300F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{50305C56-3506-426A-9490-D1BCFFFE2880}"/>
+    <workbookView xWindow="11796" yWindow="5748" windowWidth="17280" windowHeight="8964" xr2:uid="{50305C56-3506-426A-9490-D1BCFFFE2880}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="67">
   <si>
     <t>so-tensorflow</t>
   </si>
@@ -233,6 +233,9 @@
   </si>
   <si>
     <t>Check map_location only takes one argument, if it takes two remap to second  specified argument</t>
+  </si>
+  <si>
+    <t>ID for study</t>
   </si>
 </sst>
 </file>
@@ -672,443 +675,491 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D486027-A6A6-4557-9CAE-0CEFC0E0B330}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" customWidth="1"/>
-    <col min="2" max="2" width="56.21875" customWidth="1"/>
-    <col min="3" max="3" width="16.21875" customWidth="1"/>
-    <col min="4" max="4" width="53.33203125" customWidth="1"/>
-    <col min="5" max="5" width="0.21875" customWidth="1"/>
-    <col min="6" max="6" width="11.21875" customWidth="1"/>
-    <col min="9" max="9" width="25.88671875" customWidth="1"/>
-    <col min="10" max="10" width="61.5546875" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="56.21875" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" customWidth="1"/>
+    <col min="5" max="5" width="53.33203125" customWidth="1"/>
+    <col min="6" max="6" width="0.21875" customWidth="1"/>
+    <col min="7" max="7" width="11.21875" customWidth="1"/>
+    <col min="10" max="10" width="59.21875" customWidth="1"/>
+    <col min="11" max="11" width="61.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="C2" s="3">
-        <v>0</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="1">
-        <v>3</v>
-      </c>
-      <c r="G2" s="13"/>
-      <c r="I2" t="s">
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1">
+        <v>3</v>
+      </c>
+      <c r="H2" s="13"/>
+      <c r="J2" t="s">
         <v>44</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="5" t="s">
+    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="3">
+      <c r="D3" s="3">
         <v>1</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>46</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="5" t="s">
+    <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="1">
-        <v>3</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="G4" s="1">
+        <v>3</v>
+      </c>
+      <c r="J4" t="s">
         <v>48</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="8" t="s">
+    <row r="5" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="9">
-        <v>0</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>18</v>
+      <c r="D5" s="9">
+        <v>0</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="1">
-        <v>3</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="F5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="1">
+        <v>3</v>
+      </c>
+      <c r="J5" t="s">
         <v>50</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="K5" s="14" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="3">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="10">
-        <v>3</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="G6" s="10">
+        <v>3</v>
+      </c>
+      <c r="J6" t="s">
         <v>52</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="K6" s="14" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="3">
+      <c r="D7" s="3">
         <v>1</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="G7" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="3">
+      <c r="D8" s="3">
         <v>1</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="10">
-        <v>3</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="G8" s="10">
+        <v>3</v>
+      </c>
+      <c r="J8" t="s">
         <v>54</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="3">
-        <v>0</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="10">
-        <v>3</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="G9" s="10">
+        <v>3</v>
+      </c>
+      <c r="J9" t="s">
         <v>56</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="2" t="s">
+    <row r="10" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="3">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="10">
-        <v>3</v>
-      </c>
-      <c r="I10" s="15" t="s">
+      <c r="G10" s="10">
+        <v>3</v>
+      </c>
+      <c r="J10" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="3">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="G11" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="3">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="1">
-        <v>3</v>
-      </c>
-      <c r="I12" t="s">
+      <c r="G12" s="1">
+        <v>3</v>
+      </c>
+      <c r="J12" t="s">
         <v>60</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="2" t="s">
+    <row r="13" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="3">
-        <v>0</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="1">
-        <v>3</v>
-      </c>
-      <c r="I13" t="s">
+      <c r="G13" s="1">
+        <v>3</v>
+      </c>
+      <c r="J13" t="s">
         <v>62</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="3">
+      <c r="D14" s="3">
         <v>1</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>35</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="10">
-        <v>3</v>
-      </c>
-      <c r="I14" t="s">
+      <c r="H14" s="10">
+        <v>3</v>
+      </c>
+      <c r="J14" t="s">
         <v>64</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="12" t="s">
+    <row r="15" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="3">
+      <c r="D15" s="3">
         <v>1</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>37</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="G15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="3">
+      <c r="D16" s="3">
         <v>1</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="E16" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="F16" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="10">
+      <c r="H16" s="10">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{9F32EEFD-9952-44B5-9A55-FEE7FB26D36D}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{E8FE1926-2BA7-413F-9D48-91AB3AC97263}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{6E3A92AF-E7D1-4112-837A-F3306DB3195F}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{2EDEF199-8D88-4EF5-88FC-40B252A21543}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{4473FB8D-4251-44A7-80FA-C71647CE5D27}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{4A76E0A1-E000-4349-A0FF-AEC5B0C8A7AD}"/>
-    <hyperlink ref="B8" r:id="rId7" xr:uid="{EB8B04FE-5DFD-4D3C-84FA-825D31386BAB}"/>
-    <hyperlink ref="B9" r:id="rId8" xr:uid="{DE57B15A-CF81-4263-ADBA-C227C683DEA9}"/>
-    <hyperlink ref="B10" r:id="rId9" xr:uid="{99567DBD-C430-48A6-954E-EF426A9E9682}"/>
-    <hyperlink ref="B11" r:id="rId10" xr:uid="{627809DA-1421-4A30-A5F8-CCF41458450E}"/>
-    <hyperlink ref="B12" r:id="rId11" xr:uid="{2E53324D-9999-4859-AAB4-A3D85878FB76}"/>
-    <hyperlink ref="B13" r:id="rId12" xr:uid="{C9062849-FC51-451C-9FE0-131F347D3745}"/>
-    <hyperlink ref="B14" r:id="rId13" xr:uid="{FA420AA9-8552-4CDD-BBB5-F42509B7E553}"/>
-    <hyperlink ref="B15" r:id="rId14" xr:uid="{C5CD686A-1550-42AA-BC6A-F51039D638C5}"/>
-    <hyperlink ref="B16" r:id="rId15" xr:uid="{C9EED821-5573-4E22-AF9D-80EBA6A03435}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{9F32EEFD-9952-44B5-9A55-FEE7FB26D36D}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{E8FE1926-2BA7-413F-9D48-91AB3AC97263}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{6E3A92AF-E7D1-4112-837A-F3306DB3195F}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{2EDEF199-8D88-4EF5-88FC-40B252A21543}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{4473FB8D-4251-44A7-80FA-C71647CE5D27}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{4A76E0A1-E000-4349-A0FF-AEC5B0C8A7AD}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{EB8B04FE-5DFD-4D3C-84FA-825D31386BAB}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{DE57B15A-CF81-4263-ADBA-C227C683DEA9}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{99567DBD-C430-48A6-954E-EF426A9E9682}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{627809DA-1421-4A30-A5F8-CCF41458450E}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{2E53324D-9999-4859-AAB4-A3D85878FB76}"/>
+    <hyperlink ref="C13" r:id="rId12" xr:uid="{C9062849-FC51-451C-9FE0-131F347D3745}"/>
+    <hyperlink ref="C14" r:id="rId13" xr:uid="{FA420AA9-8552-4CDD-BBB5-F42509B7E553}"/>
+    <hyperlink ref="C15" r:id="rId14" xr:uid="{C5CD686A-1550-42AA-BC6A-F51039D638C5}"/>
+    <hyperlink ref="C16" r:id="rId15" xr:uid="{C9EED821-5573-4E22-AF9D-80EBA6A03435}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>

</xml_diff>

<commit_message>
added bug fix for softmax
added bug fix for soft max
</commit_message>
<xml_diff>
--- a/API Faults Taxonomy.xlsx
+++ b/API Faults Taxonomy.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wilso\OneDrive\Documents\Final Year Project\DL-BUG-FINDER\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barry\workspace\700\DL-BUG-FINDER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CFD8783-2A43-43BB-B29F-12C920738089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1FE854B-A37B-490E-9481-4B1E51395316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11265" xr2:uid="{50305C56-3506-426A-9490-D1BCFFFE2880}"/>
+    <workbookView minimized="1" xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{50305C56-3506-426A-9490-D1BCFFFE2880}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="132">
   <si>
     <t>so-tensorflow</t>
   </si>
@@ -429,6 +429,9 @@
   </si>
   <si>
     <t>Using soft-max and cross-entropy when you should just use softmax_cross_entropy_with_logits</t>
+  </si>
+  <si>
+    <t>199k</t>
   </si>
 </sst>
 </file>
@@ -895,8 +898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D486027-A6A6-4557-9CAE-0CEFC0E0B330}">
   <dimension ref="A1:W26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1658,6 +1661,12 @@
       </c>
       <c r="J26" t="s">
         <v>130</v>
+      </c>
+      <c r="L26">
+        <v>409</v>
+      </c>
+      <c r="M26" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>